<commit_message>
add annual energy simulator
</commit_message>
<xml_diff>
--- a/PvPlantPlanner/Docs/UnitTestsExamples.xlsx
+++ b/PvPlantPlanner/Docs/UnitTestsExamples.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikola.koprivica\Documents\0_MyDoc\PvPlantPlanner\PvPlantPlanner\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C197C6B9-0B29-4417-BFFC-C3A043DA3CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B8A639-A7DD-4CA3-84D3-759CA5584ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="1" xr2:uid="{CC43E566-94BC-4A10-953F-51F79849A741}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="69">
   <si>
     <t>rated Power</t>
   </si>
@@ -361,6 +361,15 @@
       <t xml:space="preserve"> + -30</t>
     </r>
   </si>
+  <si>
+    <t>SellingAlways_DynamicHighProduction_WithoutStorage_DynamicMarketPriceWithNegative</t>
+  </si>
+  <si>
+    <t>- Inf</t>
+  </si>
+  <si>
+    <t>SellingWhenNoNegative_DynamicHighProduction_WithoutStorage_DynamicMarketPriceWithNegative</t>
+  </si>
 </sst>
 </file>
 
@@ -511,7 +520,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -592,6 +601,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2676,10 +2688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3004405F-278A-41B0-B16A-948CDB79AC5D}">
-  <dimension ref="A1:S202"/>
+  <dimension ref="A1:S272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="R199" sqref="R199"/>
+    <sheetView tabSelected="1" topLeftCell="A240" workbookViewId="0">
+      <selection activeCell="M257" sqref="M257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8550,6 +8562,1968 @@
         <v>510</v>
       </c>
     </row>
+    <row r="208" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F208" s="26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="209" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="210" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A210" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B210" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C210" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D210" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E210" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="M210" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N210" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O210" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="P210" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q210" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="R210" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="S210" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="211" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A211" s="25">
+        <v>0</v>
+      </c>
+      <c r="B211" s="25">
+        <v>0</v>
+      </c>
+      <c r="C211" s="25">
+        <v>30</v>
+      </c>
+      <c r="D211" s="7">
+        <f>B211-C211</f>
+        <v>-30</v>
+      </c>
+      <c r="E211" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="M211" s="7">
+        <v>0</v>
+      </c>
+      <c r="N211" s="25">
+        <f xml:space="preserve"> M211*E211</f>
+        <v>0</v>
+      </c>
+      <c r="O211" s="7">
+        <v>30</v>
+      </c>
+      <c r="P211" s="25">
+        <f>O211*$J$145</f>
+        <v>3</v>
+      </c>
+      <c r="Q211" s="24"/>
+      <c r="R211" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A212" s="25">
+        <v>1</v>
+      </c>
+      <c r="B212" s="25">
+        <v>0</v>
+      </c>
+      <c r="C212" s="25">
+        <v>30</v>
+      </c>
+      <c r="D212" s="7">
+        <f t="shared" ref="D212:D234" si="26">B212-C212</f>
+        <v>-30</v>
+      </c>
+      <c r="E212" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G212" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M212" s="7">
+        <v>0</v>
+      </c>
+      <c r="N212" s="25">
+        <f t="shared" ref="N212:N234" si="27" xml:space="preserve"> M212*E212</f>
+        <v>0</v>
+      </c>
+      <c r="O212" s="7">
+        <v>30</v>
+      </c>
+      <c r="P212" s="25">
+        <f t="shared" ref="P212:P234" si="28">O212*$J$145</f>
+        <v>3</v>
+      </c>
+      <c r="Q212" s="24"/>
+      <c r="R212" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A213" s="25">
+        <v>2</v>
+      </c>
+      <c r="B213" s="25">
+        <v>0</v>
+      </c>
+      <c r="C213" s="25">
+        <v>30</v>
+      </c>
+      <c r="D213" s="7">
+        <f t="shared" si="26"/>
+        <v>-30</v>
+      </c>
+      <c r="E213" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G213" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J213" s="15">
+        <v>150</v>
+      </c>
+      <c r="K213" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M213" s="7">
+        <v>0</v>
+      </c>
+      <c r="N213" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O213" s="7">
+        <v>30</v>
+      </c>
+      <c r="P213" s="25">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="R213" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A214" s="25">
+        <v>3</v>
+      </c>
+      <c r="B214" s="25">
+        <v>0</v>
+      </c>
+      <c r="C214" s="25">
+        <v>30</v>
+      </c>
+      <c r="D214" s="7">
+        <f t="shared" si="26"/>
+        <v>-30</v>
+      </c>
+      <c r="E214" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="M214" s="7">
+        <v>0</v>
+      </c>
+      <c r="N214" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O214" s="7">
+        <v>30</v>
+      </c>
+      <c r="P214" s="25">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="R214" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A215" s="25">
+        <v>4</v>
+      </c>
+      <c r="B215" s="25">
+        <v>5</v>
+      </c>
+      <c r="C215" s="25">
+        <v>30</v>
+      </c>
+      <c r="D215" s="7">
+        <f t="shared" si="26"/>
+        <v>-25</v>
+      </c>
+      <c r="E215" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G215" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J215" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="K215" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M215" s="7">
+        <v>0</v>
+      </c>
+      <c r="N215" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O215" s="7">
+        <v>25</v>
+      </c>
+      <c r="P215" s="25">
+        <f t="shared" si="28"/>
+        <v>2.5</v>
+      </c>
+      <c r="R215" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A216" s="25">
+        <v>5</v>
+      </c>
+      <c r="B216" s="25">
+        <v>40</v>
+      </c>
+      <c r="C216" s="25">
+        <v>30</v>
+      </c>
+      <c r="D216" s="7">
+        <f t="shared" si="26"/>
+        <v>10</v>
+      </c>
+      <c r="E216" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M216" s="7">
+        <v>10</v>
+      </c>
+      <c r="N216" s="25">
+        <f t="shared" si="27"/>
+        <v>1</v>
+      </c>
+      <c r="O216" s="7">
+        <v>0</v>
+      </c>
+      <c r="P216" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R216" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A217" s="25">
+        <v>6</v>
+      </c>
+      <c r="B217" s="25">
+        <v>120</v>
+      </c>
+      <c r="C217" s="25">
+        <v>30</v>
+      </c>
+      <c r="D217" s="7">
+        <f t="shared" si="26"/>
+        <v>90</v>
+      </c>
+      <c r="E217" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M217" s="7">
+        <v>90</v>
+      </c>
+      <c r="N217" s="25">
+        <f t="shared" si="27"/>
+        <v>4.05</v>
+      </c>
+      <c r="O217" s="7">
+        <v>0</v>
+      </c>
+      <c r="P217" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R217" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A218" s="25">
+        <v>7</v>
+      </c>
+      <c r="B218" s="25">
+        <v>220</v>
+      </c>
+      <c r="C218" s="25">
+        <v>30</v>
+      </c>
+      <c r="D218" s="7">
+        <f t="shared" si="26"/>
+        <v>190</v>
+      </c>
+      <c r="E218" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="M218" s="7">
+        <v>150</v>
+      </c>
+      <c r="N218" s="25">
+        <f t="shared" si="27"/>
+        <v>12</v>
+      </c>
+      <c r="O218" s="7">
+        <v>0</v>
+      </c>
+      <c r="P218" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R218" s="7">
+        <v>0</v>
+      </c>
+      <c r="S218" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="219" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A219" s="25">
+        <v>8</v>
+      </c>
+      <c r="B219" s="25">
+        <v>200</v>
+      </c>
+      <c r="C219" s="25">
+        <v>30</v>
+      </c>
+      <c r="D219" s="7">
+        <f t="shared" si="26"/>
+        <v>170</v>
+      </c>
+      <c r="E219" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M219" s="7">
+        <v>150</v>
+      </c>
+      <c r="N219" s="25">
+        <f t="shared" si="27"/>
+        <v>10.500000000000002</v>
+      </c>
+      <c r="O219" s="7">
+        <v>0</v>
+      </c>
+      <c r="P219" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R219" s="7">
+        <v>0</v>
+      </c>
+      <c r="S219" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="220" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A220" s="25">
+        <v>9</v>
+      </c>
+      <c r="B220" s="25">
+        <v>480</v>
+      </c>
+      <c r="C220" s="25">
+        <v>30</v>
+      </c>
+      <c r="D220" s="7">
+        <f t="shared" si="26"/>
+        <v>450</v>
+      </c>
+      <c r="E220" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="M220" s="7">
+        <v>150</v>
+      </c>
+      <c r="N220" s="25">
+        <f t="shared" si="27"/>
+        <v>4.5</v>
+      </c>
+      <c r="O220" s="7">
+        <v>0</v>
+      </c>
+      <c r="P220" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R220" s="7">
+        <v>0</v>
+      </c>
+      <c r="S220" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="221" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A221" s="25">
+        <v>10</v>
+      </c>
+      <c r="B221" s="25">
+        <v>500</v>
+      </c>
+      <c r="C221" s="25">
+        <v>30</v>
+      </c>
+      <c r="D221" s="7">
+        <f t="shared" si="26"/>
+        <v>470</v>
+      </c>
+      <c r="E221" s="7">
+        <v>-0.01</v>
+      </c>
+      <c r="G221" s="16"/>
+      <c r="M221" s="7">
+        <v>150</v>
+      </c>
+      <c r="N221" s="25">
+        <f t="shared" si="27"/>
+        <v>-1.5</v>
+      </c>
+      <c r="O221" s="7">
+        <v>0</v>
+      </c>
+      <c r="P221" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R221" s="7">
+        <v>0</v>
+      </c>
+      <c r="S221" s="7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="222" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A222" s="25">
+        <v>11</v>
+      </c>
+      <c r="B222" s="25">
+        <v>500</v>
+      </c>
+      <c r="C222" s="25">
+        <v>30</v>
+      </c>
+      <c r="D222" s="7">
+        <f t="shared" si="26"/>
+        <v>470</v>
+      </c>
+      <c r="E222" s="7">
+        <v>-0.02</v>
+      </c>
+      <c r="M222" s="7">
+        <v>150</v>
+      </c>
+      <c r="N222" s="25">
+        <f t="shared" si="27"/>
+        <v>-3</v>
+      </c>
+      <c r="O222" s="7">
+        <v>0</v>
+      </c>
+      <c r="P222" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R222" s="7">
+        <v>0</v>
+      </c>
+      <c r="S222" s="7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="223" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A223" s="25">
+        <v>12</v>
+      </c>
+      <c r="B223" s="25">
+        <v>160</v>
+      </c>
+      <c r="C223" s="25">
+        <v>30</v>
+      </c>
+      <c r="D223" s="7">
+        <f t="shared" si="26"/>
+        <v>130</v>
+      </c>
+      <c r="E223" s="7">
+        <v>0</v>
+      </c>
+      <c r="M223" s="7">
+        <v>130</v>
+      </c>
+      <c r="N223" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O223" s="7">
+        <v>0</v>
+      </c>
+      <c r="P223" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R223" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A224" s="25">
+        <v>13</v>
+      </c>
+      <c r="B224" s="25">
+        <v>500</v>
+      </c>
+      <c r="C224" s="25">
+        <v>30</v>
+      </c>
+      <c r="D224" s="7">
+        <f t="shared" si="26"/>
+        <v>470</v>
+      </c>
+      <c r="E224" s="7">
+        <v>0</v>
+      </c>
+      <c r="M224" s="7">
+        <v>150</v>
+      </c>
+      <c r="N224" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O224" s="7">
+        <v>0</v>
+      </c>
+      <c r="P224" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R224" s="7">
+        <v>0</v>
+      </c>
+      <c r="S224" s="7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="225" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A225" s="25">
+        <v>14</v>
+      </c>
+      <c r="B225" s="25">
+        <v>480</v>
+      </c>
+      <c r="C225" s="25">
+        <v>30</v>
+      </c>
+      <c r="D225" s="7">
+        <f t="shared" si="26"/>
+        <v>450</v>
+      </c>
+      <c r="E225" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="M225" s="7">
+        <v>150</v>
+      </c>
+      <c r="N225" s="25">
+        <f t="shared" si="27"/>
+        <v>1.5</v>
+      </c>
+      <c r="O225" s="7">
+        <v>0</v>
+      </c>
+      <c r="P225" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R225" s="7">
+        <v>0</v>
+      </c>
+      <c r="S225" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="226" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A226" s="25">
+        <v>15</v>
+      </c>
+      <c r="B226" s="25">
+        <v>150</v>
+      </c>
+      <c r="C226" s="25">
+        <v>30</v>
+      </c>
+      <c r="D226" s="7">
+        <f t="shared" si="26"/>
+        <v>120</v>
+      </c>
+      <c r="E226" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="M226" s="7">
+        <v>120</v>
+      </c>
+      <c r="N226" s="25">
+        <f t="shared" si="27"/>
+        <v>2.4</v>
+      </c>
+      <c r="O226" s="7">
+        <v>0</v>
+      </c>
+      <c r="P226" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R226" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A227" s="25">
+        <v>16</v>
+      </c>
+      <c r="B227" s="25">
+        <v>140</v>
+      </c>
+      <c r="C227" s="25">
+        <v>30</v>
+      </c>
+      <c r="D227" s="7">
+        <f t="shared" si="26"/>
+        <v>110</v>
+      </c>
+      <c r="E227" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G227" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I227" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="J227" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M227" s="7">
+        <v>110</v>
+      </c>
+      <c r="N227" s="25">
+        <f t="shared" si="27"/>
+        <v>11</v>
+      </c>
+      <c r="O227" s="7">
+        <v>0</v>
+      </c>
+      <c r="P227" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R227" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A228" s="25">
+        <v>17</v>
+      </c>
+      <c r="B228" s="25">
+        <v>190</v>
+      </c>
+      <c r="C228" s="25">
+        <v>30</v>
+      </c>
+      <c r="D228" s="7">
+        <f t="shared" si="26"/>
+        <v>160</v>
+      </c>
+      <c r="E228" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="M228" s="7">
+        <v>150</v>
+      </c>
+      <c r="N228" s="25">
+        <f t="shared" si="27"/>
+        <v>16.5</v>
+      </c>
+      <c r="O228" s="7">
+        <v>0</v>
+      </c>
+      <c r="P228" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R228" s="7">
+        <v>0</v>
+      </c>
+      <c r="S228" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A229" s="25">
+        <v>18</v>
+      </c>
+      <c r="B229" s="25">
+        <v>80</v>
+      </c>
+      <c r="C229" s="25">
+        <v>30</v>
+      </c>
+      <c r="D229" s="7">
+        <f t="shared" si="26"/>
+        <v>50</v>
+      </c>
+      <c r="E229" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M229" s="7">
+        <v>50</v>
+      </c>
+      <c r="N229" s="25">
+        <f t="shared" si="27"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="O229" s="7">
+        <v>0</v>
+      </c>
+      <c r="P229" s="25">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="R229" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A230" s="25">
+        <v>19</v>
+      </c>
+      <c r="B230" s="25">
+        <v>20</v>
+      </c>
+      <c r="C230" s="25">
+        <v>30</v>
+      </c>
+      <c r="D230" s="7">
+        <f t="shared" si="26"/>
+        <v>-10</v>
+      </c>
+      <c r="E230" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="M230" s="7">
+        <v>0</v>
+      </c>
+      <c r="N230" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O230" s="7">
+        <v>10</v>
+      </c>
+      <c r="P230" s="25">
+        <f t="shared" si="28"/>
+        <v>1</v>
+      </c>
+      <c r="Q230" s="24"/>
+      <c r="R230" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A231" s="25">
+        <v>20</v>
+      </c>
+      <c r="B231" s="25">
+        <v>0</v>
+      </c>
+      <c r="C231" s="25">
+        <v>30</v>
+      </c>
+      <c r="D231" s="7">
+        <f t="shared" si="26"/>
+        <v>-30</v>
+      </c>
+      <c r="E231" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="M231" s="7">
+        <v>0</v>
+      </c>
+      <c r="N231" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O231" s="7">
+        <v>30</v>
+      </c>
+      <c r="P231" s="25">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="Q231" s="24"/>
+      <c r="R231" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A232" s="25">
+        <v>21</v>
+      </c>
+      <c r="B232" s="25">
+        <v>0</v>
+      </c>
+      <c r="C232" s="25">
+        <v>30</v>
+      </c>
+      <c r="D232" s="7">
+        <f t="shared" si="26"/>
+        <v>-30</v>
+      </c>
+      <c r="E232" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="M232" s="7">
+        <v>0</v>
+      </c>
+      <c r="N232" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O232" s="7">
+        <v>30</v>
+      </c>
+      <c r="P232" s="25">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="Q232" s="24"/>
+      <c r="R232" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A233" s="25">
+        <v>22</v>
+      </c>
+      <c r="B233" s="25">
+        <v>0</v>
+      </c>
+      <c r="C233" s="25">
+        <v>30</v>
+      </c>
+      <c r="D233" s="7">
+        <f t="shared" si="26"/>
+        <v>-30</v>
+      </c>
+      <c r="E233" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="M233" s="7">
+        <v>0</v>
+      </c>
+      <c r="N233" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O233" s="7">
+        <v>30</v>
+      </c>
+      <c r="P233" s="25">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="Q233" s="28"/>
+      <c r="R233" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="25">
+        <v>23</v>
+      </c>
+      <c r="B234" s="25">
+        <v>0</v>
+      </c>
+      <c r="C234" s="25">
+        <v>30</v>
+      </c>
+      <c r="D234" s="7">
+        <f t="shared" si="26"/>
+        <v>-30</v>
+      </c>
+      <c r="E234" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="M234" s="7">
+        <v>0</v>
+      </c>
+      <c r="N234" s="25">
+        <f t="shared" si="27"/>
+        <v>0</v>
+      </c>
+      <c r="O234" s="7">
+        <v>30</v>
+      </c>
+      <c r="P234" s="25">
+        <f t="shared" si="28"/>
+        <v>3</v>
+      </c>
+      <c r="R234" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M235" s="20">
+        <f>SUM(M211:M234)</f>
+        <v>1710</v>
+      </c>
+      <c r="N235" s="20">
+        <f t="shared" ref="N235:P235" si="29">SUM(N211:N234)</f>
+        <v>65.95</v>
+      </c>
+      <c r="O235" s="20">
+        <f t="shared" si="29"/>
+        <v>275</v>
+      </c>
+      <c r="P235" s="20">
+        <f t="shared" si="29"/>
+        <v>27.5</v>
+      </c>
+      <c r="Q235" s="21"/>
+      <c r="R235" s="17">
+        <v>0</v>
+      </c>
+      <c r="S235" s="23">
+        <f>SUM(S211:S234)</f>
+        <v>1630</v>
+      </c>
+    </row>
+    <row r="236" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q236" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="237" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q237" s="7">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="243" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="F243" s="26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="244" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="245" spans="1:19" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A245" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B245" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C245" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D245" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E245" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="M245" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N245" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="O245" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="P245" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q245" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="R245" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="S245" s="22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="246" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A246" s="25">
+        <v>0</v>
+      </c>
+      <c r="B246" s="25">
+        <v>0</v>
+      </c>
+      <c r="C246" s="25">
+        <v>30</v>
+      </c>
+      <c r="D246" s="7">
+        <f>B246-C246</f>
+        <v>-30</v>
+      </c>
+      <c r="E246" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="M246" s="7">
+        <v>0</v>
+      </c>
+      <c r="N246" s="25">
+        <f xml:space="preserve"> M246*E246</f>
+        <v>0</v>
+      </c>
+      <c r="O246" s="7">
+        <v>30</v>
+      </c>
+      <c r="P246" s="25">
+        <f>O246*$J$145</f>
+        <v>3</v>
+      </c>
+      <c r="Q246" s="24"/>
+      <c r="R246" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A247" s="25">
+        <v>1</v>
+      </c>
+      <c r="B247" s="25">
+        <v>0</v>
+      </c>
+      <c r="C247" s="25">
+        <v>30</v>
+      </c>
+      <c r="D247" s="7">
+        <f t="shared" ref="D247:D269" si="30">B247-C247</f>
+        <v>-30</v>
+      </c>
+      <c r="E247" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G247" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="M247" s="7">
+        <v>0</v>
+      </c>
+      <c r="N247" s="25">
+        <f t="shared" ref="N247:N269" si="31" xml:space="preserve"> M247*E247</f>
+        <v>0</v>
+      </c>
+      <c r="O247" s="7">
+        <v>30</v>
+      </c>
+      <c r="P247" s="25">
+        <f t="shared" ref="P247:P269" si="32">O247*$J$145</f>
+        <v>3</v>
+      </c>
+      <c r="Q247" s="24"/>
+      <c r="R247" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A248" s="25">
+        <v>2</v>
+      </c>
+      <c r="B248" s="25">
+        <v>0</v>
+      </c>
+      <c r="C248" s="25">
+        <v>30</v>
+      </c>
+      <c r="D248" s="7">
+        <f t="shared" si="30"/>
+        <v>-30</v>
+      </c>
+      <c r="E248" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G248" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J248" s="15">
+        <v>150</v>
+      </c>
+      <c r="K248" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="M248" s="7">
+        <v>0</v>
+      </c>
+      <c r="N248" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O248" s="7">
+        <v>30</v>
+      </c>
+      <c r="P248" s="25">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="R248" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A249" s="25">
+        <v>3</v>
+      </c>
+      <c r="B249" s="25">
+        <v>0</v>
+      </c>
+      <c r="C249" s="25">
+        <v>30</v>
+      </c>
+      <c r="D249" s="7">
+        <f t="shared" si="30"/>
+        <v>-30</v>
+      </c>
+      <c r="E249" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="M249" s="7">
+        <v>0</v>
+      </c>
+      <c r="N249" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O249" s="7">
+        <v>30</v>
+      </c>
+      <c r="P249" s="25">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="R249" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="250" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A250" s="25">
+        <v>4</v>
+      </c>
+      <c r="B250" s="25">
+        <v>5</v>
+      </c>
+      <c r="C250" s="25">
+        <v>30</v>
+      </c>
+      <c r="D250" s="7">
+        <f t="shared" si="30"/>
+        <v>-25</v>
+      </c>
+      <c r="E250" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G250" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J250" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="K250" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M250" s="7">
+        <v>0</v>
+      </c>
+      <c r="N250" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O250" s="7">
+        <v>25</v>
+      </c>
+      <c r="P250" s="25">
+        <f t="shared" si="32"/>
+        <v>2.5</v>
+      </c>
+      <c r="R250" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="251" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A251" s="25">
+        <v>5</v>
+      </c>
+      <c r="B251" s="25">
+        <v>40</v>
+      </c>
+      <c r="C251" s="25">
+        <v>30</v>
+      </c>
+      <c r="D251" s="7">
+        <f t="shared" si="30"/>
+        <v>10</v>
+      </c>
+      <c r="E251" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="M251" s="7">
+        <v>10</v>
+      </c>
+      <c r="N251" s="25">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="O251" s="7">
+        <v>0</v>
+      </c>
+      <c r="P251" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R251" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="252" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A252" s="25">
+        <v>6</v>
+      </c>
+      <c r="B252" s="25">
+        <v>120</v>
+      </c>
+      <c r="C252" s="25">
+        <v>30</v>
+      </c>
+      <c r="D252" s="7">
+        <f t="shared" si="30"/>
+        <v>90</v>
+      </c>
+      <c r="E252" s="7">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="M252" s="7">
+        <v>90</v>
+      </c>
+      <c r="N252" s="25">
+        <f t="shared" si="31"/>
+        <v>4.05</v>
+      </c>
+      <c r="O252" s="7">
+        <v>0</v>
+      </c>
+      <c r="P252" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R252" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A253" s="25">
+        <v>7</v>
+      </c>
+      <c r="B253" s="25">
+        <v>220</v>
+      </c>
+      <c r="C253" s="25">
+        <v>30</v>
+      </c>
+      <c r="D253" s="7">
+        <f t="shared" si="30"/>
+        <v>190</v>
+      </c>
+      <c r="E253" s="7">
+        <v>0.08</v>
+      </c>
+      <c r="M253" s="7">
+        <v>150</v>
+      </c>
+      <c r="N253" s="25">
+        <f t="shared" si="31"/>
+        <v>12</v>
+      </c>
+      <c r="O253" s="7">
+        <v>0</v>
+      </c>
+      <c r="P253" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R253" s="7">
+        <v>0</v>
+      </c>
+      <c r="S253" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="254" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A254" s="25">
+        <v>8</v>
+      </c>
+      <c r="B254" s="25">
+        <v>200</v>
+      </c>
+      <c r="C254" s="25">
+        <v>30</v>
+      </c>
+      <c r="D254" s="7">
+        <f t="shared" si="30"/>
+        <v>170</v>
+      </c>
+      <c r="E254" s="7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="M254" s="7">
+        <v>150</v>
+      </c>
+      <c r="N254" s="25">
+        <f t="shared" si="31"/>
+        <v>10.500000000000002</v>
+      </c>
+      <c r="O254" s="7">
+        <v>0</v>
+      </c>
+      <c r="P254" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R254" s="7">
+        <v>0</v>
+      </c>
+      <c r="S254" s="7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="255" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A255" s="25">
+        <v>9</v>
+      </c>
+      <c r="B255" s="25">
+        <v>480</v>
+      </c>
+      <c r="C255" s="25">
+        <v>30</v>
+      </c>
+      <c r="D255" s="7">
+        <f t="shared" si="30"/>
+        <v>450</v>
+      </c>
+      <c r="E255" s="7">
+        <v>0.03</v>
+      </c>
+      <c r="M255" s="7">
+        <v>150</v>
+      </c>
+      <c r="N255" s="25">
+        <f t="shared" si="31"/>
+        <v>4.5</v>
+      </c>
+      <c r="O255" s="7">
+        <v>0</v>
+      </c>
+      <c r="P255" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R255" s="7">
+        <v>0</v>
+      </c>
+      <c r="S255" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="256" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A256" s="25">
+        <v>10</v>
+      </c>
+      <c r="B256" s="25">
+        <v>500</v>
+      </c>
+      <c r="C256" s="25">
+        <v>30</v>
+      </c>
+      <c r="D256" s="7">
+        <f t="shared" si="30"/>
+        <v>470</v>
+      </c>
+      <c r="E256" s="7">
+        <v>-0.01</v>
+      </c>
+      <c r="G256" s="16"/>
+      <c r="M256" s="7">
+        <v>0</v>
+      </c>
+      <c r="N256" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O256" s="7">
+        <v>0</v>
+      </c>
+      <c r="P256" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R256" s="7">
+        <v>0</v>
+      </c>
+      <c r="S256" s="7">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A257" s="25">
+        <v>11</v>
+      </c>
+      <c r="B257" s="25">
+        <v>500</v>
+      </c>
+      <c r="C257" s="25">
+        <v>30</v>
+      </c>
+      <c r="D257" s="7">
+        <f t="shared" si="30"/>
+        <v>470</v>
+      </c>
+      <c r="E257" s="7">
+        <v>-0.02</v>
+      </c>
+      <c r="M257" s="7">
+        <v>0</v>
+      </c>
+      <c r="N257" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O257" s="7">
+        <v>0</v>
+      </c>
+      <c r="P257" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R257" s="7">
+        <v>0</v>
+      </c>
+      <c r="S257" s="7">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A258" s="25">
+        <v>12</v>
+      </c>
+      <c r="B258" s="25">
+        <v>160</v>
+      </c>
+      <c r="C258" s="25">
+        <v>30</v>
+      </c>
+      <c r="D258" s="7">
+        <f t="shared" si="30"/>
+        <v>130</v>
+      </c>
+      <c r="E258" s="7">
+        <v>0</v>
+      </c>
+      <c r="M258" s="7">
+        <v>130</v>
+      </c>
+      <c r="N258" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O258" s="7">
+        <v>0</v>
+      </c>
+      <c r="P258" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R258" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A259" s="25">
+        <v>13</v>
+      </c>
+      <c r="B259" s="25">
+        <v>500</v>
+      </c>
+      <c r="C259" s="25">
+        <v>30</v>
+      </c>
+      <c r="D259" s="7">
+        <f t="shared" si="30"/>
+        <v>470</v>
+      </c>
+      <c r="E259" s="7">
+        <v>0</v>
+      </c>
+      <c r="M259" s="7">
+        <v>150</v>
+      </c>
+      <c r="N259" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O259" s="7">
+        <v>0</v>
+      </c>
+      <c r="P259" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R259" s="7">
+        <v>0</v>
+      </c>
+      <c r="S259" s="7">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A260" s="25">
+        <v>14</v>
+      </c>
+      <c r="B260" s="25">
+        <v>480</v>
+      </c>
+      <c r="C260" s="25">
+        <v>30</v>
+      </c>
+      <c r="D260" s="7">
+        <f t="shared" si="30"/>
+        <v>450</v>
+      </c>
+      <c r="E260" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="M260" s="7">
+        <v>150</v>
+      </c>
+      <c r="N260" s="25">
+        <f t="shared" si="31"/>
+        <v>1.5</v>
+      </c>
+      <c r="O260" s="7">
+        <v>0</v>
+      </c>
+      <c r="P260" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R260" s="7">
+        <v>0</v>
+      </c>
+      <c r="S260" s="7">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A261" s="25">
+        <v>15</v>
+      </c>
+      <c r="B261" s="25">
+        <v>150</v>
+      </c>
+      <c r="C261" s="25">
+        <v>30</v>
+      </c>
+      <c r="D261" s="7">
+        <f t="shared" si="30"/>
+        <v>120</v>
+      </c>
+      <c r="E261" s="7">
+        <v>0.02</v>
+      </c>
+      <c r="M261" s="7">
+        <v>120</v>
+      </c>
+      <c r="N261" s="25">
+        <f t="shared" si="31"/>
+        <v>2.4</v>
+      </c>
+      <c r="O261" s="7">
+        <v>0</v>
+      </c>
+      <c r="P261" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R261" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A262" s="25">
+        <v>16</v>
+      </c>
+      <c r="B262" s="25">
+        <v>140</v>
+      </c>
+      <c r="C262" s="25">
+        <v>30</v>
+      </c>
+      <c r="D262" s="7">
+        <f t="shared" si="30"/>
+        <v>110</v>
+      </c>
+      <c r="E262" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="G262" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="I262" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="J262" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="M262" s="7">
+        <v>110</v>
+      </c>
+      <c r="N262" s="25">
+        <f t="shared" si="31"/>
+        <v>11</v>
+      </c>
+      <c r="O262" s="7">
+        <v>0</v>
+      </c>
+      <c r="P262" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R262" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A263" s="25">
+        <v>17</v>
+      </c>
+      <c r="B263" s="25">
+        <v>190</v>
+      </c>
+      <c r="C263" s="25">
+        <v>30</v>
+      </c>
+      <c r="D263" s="7">
+        <f t="shared" si="30"/>
+        <v>160</v>
+      </c>
+      <c r="E263" s="7">
+        <v>0.11</v>
+      </c>
+      <c r="M263" s="7">
+        <v>150</v>
+      </c>
+      <c r="N263" s="25">
+        <f t="shared" si="31"/>
+        <v>16.5</v>
+      </c>
+      <c r="O263" s="7">
+        <v>0</v>
+      </c>
+      <c r="P263" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R263" s="7">
+        <v>0</v>
+      </c>
+      <c r="S263" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A264" s="25">
+        <v>18</v>
+      </c>
+      <c r="B264" s="25">
+        <v>80</v>
+      </c>
+      <c r="C264" s="25">
+        <v>30</v>
+      </c>
+      <c r="D264" s="7">
+        <f t="shared" si="30"/>
+        <v>50</v>
+      </c>
+      <c r="E264" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M264" s="7">
+        <v>50</v>
+      </c>
+      <c r="N264" s="25">
+        <f t="shared" si="31"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="O264" s="7">
+        <v>0</v>
+      </c>
+      <c r="P264" s="25">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="R264" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A265" s="25">
+        <v>19</v>
+      </c>
+      <c r="B265" s="25">
+        <v>20</v>
+      </c>
+      <c r="C265" s="25">
+        <v>30</v>
+      </c>
+      <c r="D265" s="7">
+        <f t="shared" si="30"/>
+        <v>-10</v>
+      </c>
+      <c r="E265" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="M265" s="7">
+        <v>0</v>
+      </c>
+      <c r="N265" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O265" s="7">
+        <v>10</v>
+      </c>
+      <c r="P265" s="25">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="Q265" s="24"/>
+      <c r="R265" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A266" s="25">
+        <v>20</v>
+      </c>
+      <c r="B266" s="25">
+        <v>0</v>
+      </c>
+      <c r="C266" s="25">
+        <v>30</v>
+      </c>
+      <c r="D266" s="7">
+        <f t="shared" si="30"/>
+        <v>-30</v>
+      </c>
+      <c r="E266" s="7">
+        <v>0.09</v>
+      </c>
+      <c r="M266" s="7">
+        <v>0</v>
+      </c>
+      <c r="N266" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O266" s="7">
+        <v>30</v>
+      </c>
+      <c r="P266" s="25">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="Q266" s="24"/>
+      <c r="R266" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A267" s="25">
+        <v>21</v>
+      </c>
+      <c r="B267" s="25">
+        <v>0</v>
+      </c>
+      <c r="C267" s="25">
+        <v>30</v>
+      </c>
+      <c r="D267" s="7">
+        <f t="shared" si="30"/>
+        <v>-30</v>
+      </c>
+      <c r="E267" s="7">
+        <v>0.16</v>
+      </c>
+      <c r="M267" s="7">
+        <v>0</v>
+      </c>
+      <c r="N267" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O267" s="7">
+        <v>30</v>
+      </c>
+      <c r="P267" s="25">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="Q267" s="24"/>
+      <c r="R267" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A268" s="25">
+        <v>22</v>
+      </c>
+      <c r="B268" s="25">
+        <v>0</v>
+      </c>
+      <c r="C268" s="25">
+        <v>30</v>
+      </c>
+      <c r="D268" s="7">
+        <f t="shared" si="30"/>
+        <v>-30</v>
+      </c>
+      <c r="E268" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="M268" s="7">
+        <v>0</v>
+      </c>
+      <c r="N268" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O268" s="7">
+        <v>30</v>
+      </c>
+      <c r="P268" s="25">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="Q268" s="28"/>
+      <c r="R268" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A269" s="25">
+        <v>23</v>
+      </c>
+      <c r="B269" s="25">
+        <v>0</v>
+      </c>
+      <c r="C269" s="25">
+        <v>30</v>
+      </c>
+      <c r="D269" s="7">
+        <f t="shared" si="30"/>
+        <v>-30</v>
+      </c>
+      <c r="E269" s="7">
+        <v>0.13</v>
+      </c>
+      <c r="M269" s="7">
+        <v>0</v>
+      </c>
+      <c r="N269" s="25">
+        <f t="shared" si="31"/>
+        <v>0</v>
+      </c>
+      <c r="O269" s="7">
+        <v>30</v>
+      </c>
+      <c r="P269" s="25">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="R269" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M270" s="20">
+        <f>SUM(M246:M269)</f>
+        <v>1410</v>
+      </c>
+      <c r="N270" s="20">
+        <f t="shared" ref="N270:P270" si="33">SUM(N246:N269)</f>
+        <v>70.45</v>
+      </c>
+      <c r="O270" s="20">
+        <f t="shared" si="33"/>
+        <v>275</v>
+      </c>
+      <c r="P270" s="20">
+        <f t="shared" si="33"/>
+        <v>27.5</v>
+      </c>
+      <c r="Q270" s="21"/>
+      <c r="R270" s="17">
+        <v>0</v>
+      </c>
+      <c r="S270" s="23">
+        <f>SUM(S246:S269)</f>
+        <v>1930</v>
+      </c>
+    </row>
+    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q271" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q272" s="7">
+        <v>510</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>